<commit_message>
Created Cal and integration event for 00002, corrected 00001
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA03FLMA_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA03FLMA_00001.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="8190" windowWidth="26400" windowHeight="10110" activeTab="1"/>
+    <workbookView xWindow="6330" yWindow="8190" windowWidth="26400" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="110">
   <si>
     <t>Ref Des</t>
   </si>
@@ -209,39 +209,6 @@
   </si>
   <si>
     <t>GA03FLMA-RIM01-02-CTDMOG041</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOG084</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOG028</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOG068</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOG069</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOG049</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOG012</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOG010</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOG096</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOH094</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOH018</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIM01-02-CTDMOH019</t>
   </si>
   <si>
     <t>GA03FLMA-RIS01-04-PHSENF000</t>
@@ -380,6 +347,42 @@
   </si>
   <si>
     <t>13989 / 25</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG040</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG042</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG043</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG044</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG045</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG046</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG047</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG048</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOH049</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOH050</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOH051</t>
   </si>
 </sst>
 </file>
@@ -1414,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1442,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>0</v>
@@ -1477,7 +1480,7 @@
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>55</v>
@@ -1494,7 +1497,9 @@
       <c r="F2" s="12">
         <v>0.82291666666666663</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7">
+        <v>42330</v>
+      </c>
       <c r="H2" s="3" t="s">
         <v>50</v>
       </c>
@@ -1505,7 +1510,7 @@
         <v>5165</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="11">
@@ -1535,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1560,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>1</v>
@@ -1569,7 +1574,7 @@
         <v>41</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="F1" s="23" t="s">
         <v>2</v>
@@ -1589,7 +1594,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>47</v>
@@ -1598,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F2" s="13">
         <v>1215</v>
@@ -1621,7 +1626,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>47</v>
@@ -1630,7 +1635,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F3" s="13">
         <v>1215</v>
@@ -1650,7 +1655,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>47</v>
@@ -1659,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F4" s="13">
         <v>1215</v>
@@ -1676,7 +1681,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>47</v>
@@ -1685,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F5" s="13">
         <v>1215</v>
@@ -1702,7 +1707,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>47</v>
@@ -1711,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F6" s="13">
         <v>1215</v>
@@ -1728,7 +1733,7 @@
         <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>47</v>
@@ -1737,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F7" s="13">
         <v>1215</v>
@@ -1754,7 +1759,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>47</v>
@@ -1763,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F8" s="13">
         <v>1215</v>
@@ -1783,7 +1788,7 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>47</v>
@@ -1792,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F9" s="13">
         <v>1215</v>
@@ -1812,7 +1817,7 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>47</v>
@@ -1821,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F10" s="13">
         <v>1215</v>
@@ -1841,7 +1846,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>47</v>
@@ -1850,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F11" s="13">
         <v>1215</v>
@@ -1876,10 +1881,10 @@
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>47</v>
@@ -1888,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>52</v>
@@ -1908,10 +1913,10 @@
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>47</v>
@@ -1920,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>52</v>
@@ -1934,10 +1939,10 @@
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>47</v>
@@ -1946,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>52</v>
@@ -1960,10 +1965,10 @@
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>47</v>
@@ -1972,7 +1977,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>52</v>
@@ -1986,10 +1991,10 @@
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>47</v>
@@ -1998,7 +2003,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>52</v>
@@ -2012,10 +2017,10 @@
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>47</v>
@@ -2024,7 +2029,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>52</v>
@@ -2038,10 +2043,10 @@
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>47</v>
@@ -2050,7 +2055,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>52</v>
@@ -2079,7 +2084,7 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>47</v>
@@ -2088,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F21" s="13">
         <v>428</v>
@@ -2111,7 +2116,7 @@
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>47</v>
@@ -2120,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F22" s="13">
         <v>428</v>
@@ -2140,7 +2145,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>47</v>
@@ -2149,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F23" s="13">
         <v>428</v>
@@ -2175,7 +2180,7 @@
         <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>47</v>
@@ -2184,7 +2189,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F25" s="13">
         <v>20503</v>
@@ -2207,7 +2212,7 @@
         <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>47</v>
@@ -2216,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F26" s="13">
         <v>20503</v>
@@ -2233,7 +2238,7 @@
         <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>47</v>
@@ -2242,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F27" s="13">
         <v>20503</v>
@@ -2259,7 +2264,7 @@
         <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>47</v>
@@ -2268,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F28" s="13">
         <v>20503</v>
@@ -2285,7 +2290,7 @@
         <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>47</v>
@@ -2294,7 +2299,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F29" s="13">
         <v>20503</v>
@@ -2311,7 +2316,7 @@
         <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>47</v>
@@ -2320,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F30" s="13">
         <v>20503</v>
@@ -2337,7 +2342,7 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>47</v>
@@ -2346,7 +2351,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F31" s="13">
         <v>20503</v>
@@ -2363,7 +2368,7 @@
         <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>47</v>
@@ -2372,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F32" s="13">
         <v>20503</v>
@@ -2384,12 +2389,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>47</v>
@@ -2398,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F33" s="13">
         <v>20503</v>
@@ -2410,7 +2415,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34"/>
       <c r="C34" s="14"/>
@@ -2419,12 +2424,12 @@
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
     </row>
-    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>47</v>
@@ -2433,10 +2438,10 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>5</v>
@@ -2450,13 +2455,16 @@
       <c r="J35" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K35" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>47</v>
@@ -2465,10 +2473,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>6</v>
@@ -2477,12 +2485,12 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>47</v>
@@ -2491,10 +2499,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>7</v>
@@ -2503,12 +2511,12 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>47</v>
@@ -2517,10 +2525,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>29</v>
@@ -2529,7 +2537,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39"/>
       <c r="C39" s="14"/>
@@ -2539,12 +2547,12 @@
       <c r="G39" s="13"/>
       <c r="H39" s="27"/>
     </row>
-    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>47</v>
@@ -2553,10 +2561,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>5</v>
@@ -2570,13 +2578,16 @@
       <c r="J40" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K40" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>47</v>
@@ -2585,10 +2596,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>6</v>
@@ -2597,12 +2608,12 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>47</v>
@@ -2611,10 +2622,10 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>7</v>
@@ -2623,12 +2634,12 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>47</v>
@@ -2637,10 +2648,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>29</v>
@@ -2649,7 +2660,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44"/>
       <c r="C44" s="14"/>
@@ -2659,12 +2670,12 @@
       <c r="G44" s="13"/>
       <c r="H44" s="27"/>
     </row>
-    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>47</v>
@@ -2673,10 +2684,10 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G45" s="13" t="s">
         <v>5</v>
@@ -2690,13 +2701,16 @@
       <c r="J45" s="2">
         <v>59</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K45" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>47</v>
@@ -2705,10 +2719,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>6</v>
@@ -2717,12 +2731,12 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>47</v>
@@ -2731,10 +2745,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>7</v>
@@ -2743,12 +2757,12 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>47</v>
@@ -2757,10 +2771,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>29</v>
@@ -2781,10 +2795,10 @@
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>47</v>
@@ -2793,10 +2807,10 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F50" s="25" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>5</v>
@@ -2813,10 +2827,10 @@
     </row>
     <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>47</v>
@@ -2825,10 +2839,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>6</v>
@@ -2839,10 +2853,10 @@
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>47</v>
@@ -2851,10 +2865,10 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>7</v>
@@ -2865,10 +2879,10 @@
     </row>
     <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>47</v>
@@ -2877,10 +2891,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F53" s="25" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G53" s="13" t="s">
         <v>29</v>
@@ -2901,10 +2915,10 @@
     </row>
     <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>47</v>
@@ -2913,10 +2927,10 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F55" s="25" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>5</v>
@@ -2933,10 +2947,10 @@
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>47</v>
@@ -2945,10 +2959,10 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F56" s="25" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>6</v>
@@ -2959,10 +2973,10 @@
     </row>
     <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>47</v>
@@ -2971,10 +2985,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F57" s="25" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G57" s="13" t="s">
         <v>7</v>
@@ -2985,10 +2999,10 @@
     </row>
     <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>47</v>
@@ -2997,10 +3011,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>29</v>
@@ -3021,10 +3035,10 @@
     </row>
     <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>47</v>
@@ -3033,10 +3047,10 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>5</v>
@@ -3053,10 +3067,10 @@
     </row>
     <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>47</v>
@@ -3065,10 +3079,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>6</v>
@@ -3079,10 +3093,10 @@
     </row>
     <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>47</v>
@@ -3091,10 +3105,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>7</v>
@@ -3105,10 +3119,10 @@
     </row>
     <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>47</v>
@@ -3117,10 +3131,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>29</v>
@@ -3141,22 +3155,22 @@
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D65" s="13">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
         <v>85</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D65" s="13">
-        <v>1</v>
-      </c>
-      <c r="E65" t="s">
-        <v>96</v>
-      </c>
       <c r="F65" s="25" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>5</v>
@@ -3173,22 +3187,22 @@
     </row>
     <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="B66" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D66" s="13">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D66" s="13">
-        <v>1</v>
-      </c>
-      <c r="E66" t="s">
-        <v>96</v>
-      </c>
       <c r="F66" s="25" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>6</v>
@@ -3199,22 +3213,22 @@
     </row>
     <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="B67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67" s="13">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
         <v>85</v>
       </c>
-      <c r="C67" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D67" s="13">
-        <v>1</v>
-      </c>
-      <c r="E67" t="s">
-        <v>96</v>
-      </c>
       <c r="F67" s="25" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>7</v>
@@ -3225,22 +3239,22 @@
     </row>
     <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="B68" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" s="13">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
         <v>85</v>
       </c>
-      <c r="C68" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="13">
-        <v>1</v>
-      </c>
-      <c r="E68" t="s">
-        <v>96</v>
-      </c>
       <c r="F68" s="25" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>29</v>
@@ -3261,10 +3275,10 @@
     </row>
     <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>47</v>
@@ -3273,10 +3287,10 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>5</v>
@@ -3293,10 +3307,10 @@
     </row>
     <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>47</v>
@@ -3305,10 +3319,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>6</v>
@@ -3319,10 +3333,10 @@
     </row>
     <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>47</v>
@@ -3331,10 +3345,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>7</v>
@@ -3345,10 +3359,10 @@
     </row>
     <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>47</v>
@@ -3357,10 +3371,10 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>29</v>
@@ -3381,10 +3395,10 @@
     </row>
     <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>47</v>
@@ -3393,10 +3407,10 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F75" s="26" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>5</v>
@@ -3413,10 +3427,10 @@
     </row>
     <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>47</v>
@@ -3425,10 +3439,10 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F76" s="26" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>6</v>
@@ -3439,10 +3453,10 @@
     </row>
     <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>47</v>
@@ -3451,10 +3465,10 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F77" s="26" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>7</v>
@@ -3465,10 +3479,10 @@
     </row>
     <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>47</v>
@@ -3477,10 +3491,10 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F78" s="26" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>29</v>
@@ -3501,10 +3515,10 @@
     </row>
     <row r="80" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="B80" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>47</v>
@@ -3513,10 +3527,10 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F80" s="26" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G80" s="16" t="s">
         <v>5</v>
@@ -3533,10 +3547,10 @@
     </row>
     <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>47</v>
@@ -3545,10 +3559,10 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F81" s="25" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>6</v>
@@ -3559,10 +3573,10 @@
     </row>
     <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C82" s="14" t="s">
         <v>47</v>
@@ -3571,10 +3585,10 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>7</v>
@@ -3585,10 +3599,10 @@
     </row>
     <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C83" s="14" t="s">
         <v>47</v>
@@ -3597,10 +3611,10 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>29</v>
@@ -3621,10 +3635,10 @@
     </row>
     <row r="85" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>47</v>
@@ -3633,10 +3647,10 @@
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F85" s="25" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>5</v>
@@ -3653,10 +3667,10 @@
     </row>
     <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="B86" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>47</v>
@@ -3665,10 +3679,10 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F86" s="25" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>6</v>
@@ -3679,10 +3693,10 @@
     </row>
     <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>47</v>
@@ -3691,10 +3705,10 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F87" s="25" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>7</v>
@@ -3705,10 +3719,10 @@
     </row>
     <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="B88" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>47</v>
@@ -3717,10 +3731,10 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F88" s="25" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>29</v>
@@ -3741,10 +3755,10 @@
     </row>
     <row r="90" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="B90" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>47</v>
@@ -3753,10 +3767,10 @@
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F90" s="25" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>5</v>
@@ -3773,10 +3787,10 @@
     </row>
     <row r="91" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="B91" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>47</v>
@@ -3785,10 +3799,10 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F91" s="25" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>6</v>
@@ -3799,10 +3813,10 @@
     </row>
     <row r="92" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="B92" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C92" s="14" t="s">
         <v>47</v>
@@ -3811,10 +3825,10 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F92" s="25" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>7</v>
@@ -3825,10 +3839,10 @@
     </row>
     <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="B93" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>47</v>
@@ -3837,10 +3851,10 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F93" s="25" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>29</v>
@@ -3861,10 +3875,10 @@
     </row>
     <row r="95" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>47</v>
@@ -3873,10 +3887,10 @@
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="G95" s="13"/>
       <c r="I95" s="20" t="s">
@@ -3885,10 +3899,10 @@
     </row>
     <row r="96" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>47</v>
@@ -3897,10 +3911,10 @@
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated Global Surface and Flanking mooring CC_depth
CC_depth for ADCPs on Global Surface and Flanking moorings should be
500000 (units in mm)
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA03FLMA_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA03FLMA_00001.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="8190" windowWidth="26400" windowHeight="10110"/>
+    <workbookView xWindow="6340" yWindow="8200" windowWidth="26400" windowHeight="10120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +17,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="111">
   <si>
     <t>Ref Des</t>
   </si>
@@ -383,6 +378,9 @@
   </si>
   <si>
     <t>GA03FLMA-RIM01-02-CTDMOH051</t>
+  </si>
+  <si>
+    <t>Units in mm</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1110,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1171,7 +1169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1206,7 +1204,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1417,30 +1415,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="8.7109375" style="4"/>
+    <col min="8" max="8" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13.5" style="4" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="28">
       <c r="A1" s="28" t="s">
         <v>73</v>
       </c>
@@ -1478,7 +1476,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="9" customFormat="1">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1522,7 +1520,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="9" customFormat="1">
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
       <c r="G3" s="17"/>
@@ -1542,25 +1540,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7109375" style="2"/>
+    <col min="9" max="9" width="8.6640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="24" customFormat="1" ht="28">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +1587,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="13" t="s">
         <v>56</v>
       </c>
@@ -1621,7 +1619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="13" t="s">
         <v>56</v>
       </c>
@@ -1650,7 +1648,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="13" t="s">
         <v>56</v>
       </c>
@@ -1676,7 +1674,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>56</v>
       </c>
@@ -1702,7 +1700,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="13" t="s">
         <v>56</v>
       </c>
@@ -1728,7 +1726,7 @@
         <v>9.06E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="13" t="s">
         <v>56</v>
       </c>
@@ -1754,7 +1752,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="13" t="s">
         <v>56</v>
       </c>
@@ -1783,7 +1781,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="13" t="s">
         <v>56</v>
       </c>
@@ -1812,7 +1810,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="13" t="s">
         <v>56</v>
       </c>
@@ -1841,7 +1839,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="13" t="s">
         <v>56</v>
       </c>
@@ -1870,7 +1868,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="13"/>
       <c r="B12"/>
       <c r="C12" s="14"/>
@@ -1879,7 +1877,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="13" t="s">
         <v>59</v>
       </c>
@@ -1911,7 +1909,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="13" t="s">
         <v>59</v>
       </c>
@@ -1937,7 +1935,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="13" t="s">
         <v>59</v>
       </c>
@@ -1963,7 +1961,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="13" t="s">
         <v>59</v>
       </c>
@@ -1989,7 +1987,7 @@
         <v>38502</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="13" t="s">
         <v>59</v>
       </c>
@@ -2015,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="13" t="s">
         <v>59</v>
       </c>
@@ -2041,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="13" t="s">
         <v>59</v>
       </c>
@@ -2070,7 +2068,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="13"/>
       <c r="B20"/>
       <c r="C20" s="14"/>
@@ -2079,7 +2077,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="13" t="s">
         <v>48</v>
       </c>
@@ -2111,7 +2109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="13" t="s">
         <v>48</v>
       </c>
@@ -2140,7 +2138,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="13" t="s">
         <v>48</v>
       </c>
@@ -2166,7 +2164,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="13"/>
       <c r="B24"/>
       <c r="C24" s="14"/>
@@ -2175,7 +2173,7 @@
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="13" t="s">
         <v>57</v>
       </c>
@@ -2207,7 +2205,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="13" t="s">
         <v>57</v>
       </c>
@@ -2233,7 +2231,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="13" t="s">
         <v>57</v>
       </c>
@@ -2259,7 +2257,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="13" t="s">
         <v>57</v>
       </c>
@@ -2285,7 +2283,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="13" t="s">
         <v>57</v>
       </c>
@@ -2310,8 +2308,11 @@
       <c r="H29" s="2">
         <v>500000</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="I29" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="13" t="s">
         <v>57</v>
       </c>
@@ -2337,7 +2338,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="13" t="s">
         <v>57</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="13" t="s">
         <v>57</v>
       </c>
@@ -2389,7 +2390,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="13" t="s">
         <v>57</v>
       </c>
@@ -2415,7 +2416,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="13"/>
       <c r="B34"/>
       <c r="C34" s="14"/>
@@ -2424,7 +2425,7 @@
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
     </row>
-    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="13" t="s">
         <v>98</v>
       </c>
@@ -2459,7 +2460,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="13" t="s">
         <v>98</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="13" t="s">
         <v>98</v>
       </c>
@@ -2511,7 +2512,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="13" t="s">
         <v>98</v>
       </c>
@@ -2537,7 +2538,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="13"/>
       <c r="B39"/>
       <c r="C39" s="14"/>
@@ -2547,7 +2548,7 @@
       <c r="G39" s="13"/>
       <c r="H39" s="27"/>
     </row>
-    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="13" t="s">
         <v>58</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="13" t="s">
         <v>58</v>
       </c>
@@ -2608,7 +2609,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="13" t="s">
         <v>58</v>
       </c>
@@ -2634,7 +2635,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="13" t="s">
         <v>58</v>
       </c>
@@ -2660,7 +2661,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" s="13"/>
       <c r="B44"/>
       <c r="C44" s="14"/>
@@ -2670,7 +2671,7 @@
       <c r="G44" s="13"/>
       <c r="H44" s="27"/>
     </row>
-    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" s="13" t="s">
         <v>100</v>
       </c>
@@ -2705,7 +2706,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" s="13" t="s">
         <v>100</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47" s="13" t="s">
         <v>100</v>
       </c>
@@ -2757,7 +2758,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" s="13" t="s">
         <v>100</v>
       </c>
@@ -2783,7 +2784,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="13"/>
       <c r="B49"/>
       <c r="C49" s="14"/>
@@ -2793,7 +2794,7 @@
       <c r="G49" s="13"/>
       <c r="H49" s="27"/>
     </row>
-    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="13" t="s">
         <v>101</v>
       </c>
@@ -2825,7 +2826,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="13" t="s">
         <v>101</v>
       </c>
@@ -2851,7 +2852,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="13" t="s">
         <v>101</v>
       </c>
@@ -2877,7 +2878,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="13" t="s">
         <v>101</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="13"/>
       <c r="B54"/>
       <c r="C54" s="14"/>
@@ -2913,7 +2914,7 @@
       <c r="G54" s="13"/>
       <c r="H54" s="27"/>
     </row>
-    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="13" t="s">
         <v>102</v>
       </c>
@@ -2945,7 +2946,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="13" t="s">
         <v>102</v>
       </c>
@@ -2971,7 +2972,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="13" t="s">
         <v>102</v>
       </c>
@@ -2997,7 +2998,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="13" t="s">
         <v>102</v>
       </c>
@@ -3023,7 +3024,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="13"/>
       <c r="B59"/>
       <c r="C59" s="14"/>
@@ -3033,7 +3034,7 @@
       <c r="G59" s="13"/>
       <c r="H59" s="27"/>
     </row>
-    <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="13" t="s">
         <v>103</v>
       </c>
@@ -3065,7 +3066,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="13" t="s">
         <v>103</v>
       </c>
@@ -3091,7 +3092,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="13" t="s">
         <v>103</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="13" t="s">
         <v>103</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="13"/>
       <c r="B64"/>
       <c r="C64" s="14"/>
@@ -3153,7 +3154,7 @@
       <c r="G64" s="13"/>
       <c r="H64" s="27"/>
     </row>
-    <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="13" t="s">
         <v>104</v>
       </c>
@@ -3185,7 +3186,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="13" t="s">
         <v>104</v>
       </c>
@@ -3211,7 +3212,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="13" t="s">
         <v>104</v>
       </c>
@@ -3237,7 +3238,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="13" t="s">
         <v>104</v>
       </c>
@@ -3263,7 +3264,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="13"/>
       <c r="B69"/>
       <c r="C69" s="14"/>
@@ -3273,7 +3274,7 @@
       <c r="G69" s="13"/>
       <c r="H69" s="27"/>
     </row>
-    <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="13" t="s">
         <v>105</v>
       </c>
@@ -3305,7 +3306,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="13" t="s">
         <v>105</v>
       </c>
@@ -3331,7 +3332,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="13" t="s">
         <v>105</v>
       </c>
@@ -3357,7 +3358,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="13" t="s">
         <v>105</v>
       </c>
@@ -3383,7 +3384,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="13"/>
       <c r="B74"/>
       <c r="C74" s="14"/>
@@ -3393,7 +3394,7 @@
       <c r="G74" s="13"/>
       <c r="H74" s="27"/>
     </row>
-    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="13" t="s">
         <v>106</v>
       </c>
@@ -3425,7 +3426,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="13" t="s">
         <v>106</v>
       </c>
@@ -3451,7 +3452,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="13" t="s">
         <v>106</v>
       </c>
@@ -3477,7 +3478,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="13" t="s">
         <v>106</v>
       </c>
@@ -3503,7 +3504,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="13"/>
       <c r="B79"/>
       <c r="C79" s="14"/>
@@ -3513,7 +3514,7 @@
       <c r="G79" s="13"/>
       <c r="H79" s="27"/>
     </row>
-    <row r="80" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" s="1" customFormat="1">
       <c r="A80" s="13" t="s">
         <v>107</v>
       </c>
@@ -3545,7 +3546,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="13" t="s">
         <v>107</v>
       </c>
@@ -3571,7 +3572,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="13" t="s">
         <v>107</v>
       </c>
@@ -3597,7 +3598,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="13" t="s">
         <v>107</v>
       </c>
@@ -3623,7 +3624,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="13"/>
       <c r="B84"/>
       <c r="C84" s="14"/>
@@ -3633,7 +3634,7 @@
       <c r="G84" s="13"/>
       <c r="H84" s="27"/>
     </row>
-    <row r="85" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="13" t="s">
         <v>108</v>
       </c>
@@ -3665,7 +3666,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="13" t="s">
         <v>108</v>
       </c>
@@ -3691,7 +3692,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="13" t="s">
         <v>108</v>
       </c>
@@ -3717,7 +3718,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="13" t="s">
         <v>108</v>
       </c>
@@ -3743,7 +3744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="13"/>
       <c r="B89"/>
       <c r="C89" s="14"/>
@@ -3753,7 +3754,7 @@
       <c r="G89" s="13"/>
       <c r="H89" s="27"/>
     </row>
-    <row r="90" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="13" t="s">
         <v>109</v>
       </c>
@@ -3785,7 +3786,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="13" t="s">
         <v>109</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="13" t="s">
         <v>109</v>
       </c>
@@ -3837,7 +3838,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="13" t="s">
         <v>109</v>
       </c>
@@ -3863,7 +3864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="13"/>
       <c r="B94"/>
       <c r="C94" s="14"/>
@@ -3873,7 +3874,7 @@
       <c r="G94" s="13"/>
       <c r="H94" s="27"/>
     </row>
-    <row r="95" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="13" t="s">
         <v>93</v>
       </c>
@@ -3897,7 +3898,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="13" t="s">
         <v>92</v>
       </c>
@@ -3917,7 +3918,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="14"/>
@@ -3926,7 +3927,7 @@
       <c r="F97" s="13"/>
       <c r="G97" s="13"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7">
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
       <c r="D98" s="13"/>
@@ -3934,7 +3935,7 @@
       <c r="F98" s="13"/>
       <c r="G98" s="13"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7">
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
@@ -3942,7 +3943,7 @@
       <c r="F99" s="13"/>
       <c r="G99" s="13"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
@@ -3951,7 +3952,7 @@
       <c r="F100" s="13"/>
       <c r="G100" s="13"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>
@@ -3960,7 +3961,7 @@
       <c r="F101" s="13"/>
       <c r="G101" s="13"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" s="13"/>
       <c r="B102" s="13"/>
       <c r="C102" s="13"/>

</xml_diff>

<commit_message>
GA03FLMA_00001 - fixed longitude
The wrong anchor position was recorded in the Argentine-1 cruise
report. The mooring was found on the subsequent cruise at 42°
29.64’S, 042° 52.24’W (reported as 57.74’W). Updated longitude in cal
sheet.
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA03FLMA_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA03FLMA_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6340" yWindow="8200" windowWidth="26400" windowHeight="10120" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="560" windowWidth="33980" windowHeight="16580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="112">
   <si>
     <t>Ref Des</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>42° 29.58' S</t>
-  </si>
-  <si>
-    <t>42° 57.74' W</t>
   </si>
   <si>
     <t>P0141</t>
@@ -381,6 +378,12 @@
   </si>
   <si>
     <t>Units in mm</t>
+  </si>
+  <si>
+    <t>42° 52.24' W</t>
+  </si>
+  <si>
+    <t>Wrong anchor position recovered in Argentine-1 Cruise report. Fixed here</t>
   </si>
 </sst>
 </file>
@@ -674,7 +677,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="164">
+  <cellStyleXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -839,6 +842,10 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -930,7 +937,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="164">
+  <cellStyles count="168">
     <cellStyle name="Comma 2" xfId="63"/>
     <cellStyle name="Comma 2 2" xfId="64"/>
     <cellStyle name="Comma 2 2 2" xfId="65"/>
@@ -957,6 +964,8 @@
     <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
@@ -973,6 +982,8 @@
     <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="9"/>
     <cellStyle name="Hyperlink 2 2" xfId="72"/>
     <cellStyle name="Hyperlink 2 3" xfId="73"/>
@@ -1113,14 +1124,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Read Me"/>
       <sheetName val="Moorings"/>
-      <sheetName val="Asset_Cal_Info"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1415,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1440,7 +1447,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" ht="28">
       <c r="A1" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>0</v>
@@ -1478,10 +1485,10 @@
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>47</v>
@@ -1502,22 +1509,24 @@
         <v>50</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="J2" s="3">
         <v>5165</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" s="3"/>
+        <v>59</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="M2" s="11">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
         <v>-42.493000000000002</v>
       </c>
       <c r="N2" s="11">
         <f>((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="9" customFormat="1">
@@ -1540,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1563,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>1</v>
@@ -1572,7 +1581,7 @@
         <v>41</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F1" s="23" t="s">
         <v>2</v>
@@ -1589,10 +1598,10 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>47</v>
@@ -1601,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="13">
         <v>1215</v>
@@ -1621,10 +1630,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>47</v>
@@ -1633,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F3" s="13">
         <v>1215</v>
@@ -1650,10 +1659,10 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>47</v>
@@ -1662,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="13">
         <v>1215</v>
@@ -1676,10 +1685,10 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>47</v>
@@ -1688,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F5" s="13">
         <v>1215</v>
@@ -1702,10 +1711,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>47</v>
@@ -1714,7 +1723,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="13">
         <v>1215</v>
@@ -1728,10 +1737,10 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>47</v>
@@ -1740,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="13">
         <v>1215</v>
@@ -1754,10 +1763,10 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>47</v>
@@ -1766,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" s="13">
         <v>1215</v>
@@ -1783,10 +1792,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>47</v>
@@ -1795,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" s="13">
         <v>1215</v>
@@ -1812,10 +1821,10 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>47</v>
@@ -1824,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" s="13">
         <v>1215</v>
@@ -1841,10 +1850,10 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>47</v>
@@ -1853,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" s="13">
         <v>1215</v>
@@ -1879,10 +1888,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>47</v>
@@ -1891,10 +1900,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>18</v>
@@ -1911,10 +1920,10 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>47</v>
@@ -1923,10 +1932,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>19</v>
@@ -1937,10 +1946,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>47</v>
@@ -1949,10 +1958,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>20</v>
@@ -1963,10 +1972,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>47</v>
@@ -1975,10 +1984,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>21</v>
@@ -1989,10 +1998,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>47</v>
@@ -2001,10 +2010,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>22</v>
@@ -2015,10 +2024,10 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>47</v>
@@ -2027,10 +2036,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>23</v>
@@ -2041,10 +2050,10 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>47</v>
@@ -2053,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>39</v>
@@ -2082,7 +2091,7 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>47</v>
@@ -2091,7 +2100,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F21" s="13">
         <v>428</v>
@@ -2114,7 +2123,7 @@
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>47</v>
@@ -2123,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F22" s="13">
         <v>428</v>
@@ -2132,7 +2141,7 @@
         <v>7</v>
       </c>
       <c r="H22" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>49</v>
@@ -2143,7 +2152,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>47</v>
@@ -2152,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F23" s="13">
         <v>428</v>
@@ -2161,7 +2170,7 @@
         <v>15</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2175,10 +2184,10 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>47</v>
@@ -2187,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="13">
         <v>20503</v>
@@ -2207,10 +2216,10 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>47</v>
@@ -2219,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F26" s="13">
         <v>20503</v>
@@ -2228,15 +2237,15 @@
         <v>7</v>
       </c>
       <c r="H26" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>47</v>
@@ -2245,7 +2254,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F27" s="13">
         <v>20503</v>
@@ -2259,10 +2268,10 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>47</v>
@@ -2271,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F28" s="13">
         <v>20503</v>
@@ -2280,15 +2289,15 @@
         <v>9</v>
       </c>
       <c r="H28" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>47</v>
@@ -2297,7 +2306,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F29" s="13">
         <v>20503</v>
@@ -2309,15 +2318,15 @@
         <v>500000</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>47</v>
@@ -2326,7 +2335,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F30" s="13">
         <v>20503</v>
@@ -2340,10 +2349,10 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>47</v>
@@ -2352,7 +2361,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F31" s="13">
         <v>20503</v>
@@ -2366,10 +2375,10 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>47</v>
@@ -2378,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F32" s="13">
         <v>20503</v>
@@ -2392,10 +2401,10 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>47</v>
@@ -2404,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F33" s="13">
         <v>20503</v>
@@ -2427,10 +2436,10 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>47</v>
@@ -2439,10 +2448,10 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>5</v>
@@ -2457,15 +2466,15 @@
         <v>29</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>47</v>
@@ -2474,10 +2483,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>6</v>
@@ -2488,10 +2497,10 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>47</v>
@@ -2500,24 +2509,24 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H37" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>47</v>
@@ -2526,10 +2535,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>29</v>
@@ -2550,10 +2559,10 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>47</v>
@@ -2562,10 +2571,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>5</v>
@@ -2580,15 +2589,15 @@
         <v>39</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>47</v>
@@ -2597,10 +2606,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>6</v>
@@ -2611,10 +2620,10 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>47</v>
@@ -2623,24 +2632,24 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H42" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>47</v>
@@ -2649,10 +2658,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>29</v>
@@ -2673,10 +2682,10 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>47</v>
@@ -2685,10 +2694,10 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G45" s="13" t="s">
         <v>5</v>
@@ -2703,15 +2712,15 @@
         <v>59</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>47</v>
@@ -2720,10 +2729,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>6</v>
@@ -2734,10 +2743,10 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>47</v>
@@ -2746,24 +2755,24 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H47" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>47</v>
@@ -2772,10 +2781,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>29</v>
@@ -2796,10 +2805,10 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>47</v>
@@ -2808,10 +2817,10 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F50" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>5</v>
@@ -2828,10 +2837,10 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>47</v>
@@ -2840,10 +2849,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>6</v>
@@ -2854,10 +2863,10 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>47</v>
@@ -2866,24 +2875,24 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H52" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>47</v>
@@ -2892,10 +2901,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F53" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G53" s="13" t="s">
         <v>29</v>
@@ -2916,10 +2925,10 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>47</v>
@@ -2928,10 +2937,10 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F55" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>5</v>
@@ -2948,10 +2957,10 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>47</v>
@@ -2960,10 +2969,10 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F56" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>6</v>
@@ -2974,10 +2983,10 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>47</v>
@@ -2986,24 +2995,24 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F57" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G57" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H57" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>47</v>
@@ -3012,10 +3021,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>29</v>
@@ -3036,10 +3045,10 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>47</v>
@@ -3048,10 +3057,10 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>5</v>
@@ -3068,10 +3077,10 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>47</v>
@@ -3080,10 +3089,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>6</v>
@@ -3094,10 +3103,10 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>47</v>
@@ -3106,24 +3115,24 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H62" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>47</v>
@@ -3132,10 +3141,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>29</v>
@@ -3156,10 +3165,10 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>47</v>
@@ -3168,10 +3177,10 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>5</v>
@@ -3188,10 +3197,10 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>47</v>
@@ -3200,10 +3209,10 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>6</v>
@@ -3214,10 +3223,10 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>47</v>
@@ -3226,24 +3235,24 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H67" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>47</v>
@@ -3252,10 +3261,10 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F68" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>29</v>
@@ -3276,10 +3285,10 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>47</v>
@@ -3288,10 +3297,10 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>5</v>
@@ -3308,10 +3317,10 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>47</v>
@@ -3320,10 +3329,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>6</v>
@@ -3334,10 +3343,10 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>47</v>
@@ -3346,24 +3355,24 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H72" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>47</v>
@@ -3372,10 +3381,10 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>29</v>
@@ -3396,10 +3405,10 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>47</v>
@@ -3408,10 +3417,10 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F75" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>5</v>
@@ -3428,10 +3437,10 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>47</v>
@@ -3440,10 +3449,10 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F76" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>6</v>
@@ -3454,10 +3463,10 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>47</v>
@@ -3466,24 +3475,24 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F77" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H77" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>47</v>
@@ -3492,10 +3501,10 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F78" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>29</v>
@@ -3516,10 +3525,10 @@
     </row>
     <row r="80" spans="1:10" s="1" customFormat="1">
       <c r="A80" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>47</v>
@@ -3528,10 +3537,10 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F80" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G80" s="16" t="s">
         <v>5</v>
@@ -3548,10 +3557,10 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>47</v>
@@ -3560,10 +3569,10 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F81" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>6</v>
@@ -3574,10 +3583,10 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C82" s="14" t="s">
         <v>47</v>
@@ -3586,24 +3595,24 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H82" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C83" s="14" t="s">
         <v>47</v>
@@ -3612,10 +3621,10 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>29</v>
@@ -3636,10 +3645,10 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>47</v>
@@ -3648,10 +3657,10 @@
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F85" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>5</v>
@@ -3668,10 +3677,10 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B86" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>47</v>
@@ -3680,10 +3689,10 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F86" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>6</v>
@@ -3694,10 +3703,10 @@
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B87" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>47</v>
@@ -3706,24 +3715,24 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F87" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H87" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B88" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>47</v>
@@ -3732,10 +3741,10 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F88" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>29</v>
@@ -3756,10 +3765,10 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B90" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>47</v>
@@ -3768,10 +3777,10 @@
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F90" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>5</v>
@@ -3788,10 +3797,10 @@
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B91" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>47</v>
@@ -3800,10 +3809,10 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F91" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>6</v>
@@ -3814,10 +3823,10 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C92" s="14" t="s">
         <v>47</v>
@@ -3826,24 +3835,24 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F92" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H92" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.870666666666665</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>47</v>
@@ -3852,10 +3861,10 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F93" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>29</v>
@@ -3876,34 +3885,34 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B95" t="s">
+        <v>73</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D95" s="13">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
         <v>93</v>
       </c>
-      <c r="B95" t="s">
-        <v>74</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D95" s="13">
-        <v>1</v>
-      </c>
-      <c r="E95" t="s">
-        <v>94</v>
-      </c>
       <c r="F95" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G95" s="13"/>
       <c r="I95" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>47</v>
@@ -3912,10 +3921,10 @@
         <v>1</v>
       </c>
       <c r="E96" t="s">
+        <v>94</v>
+      </c>
+      <c r="F96" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="F96" s="21" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:7">

</xml_diff>